<commit_message>
update rar ref table
</commit_message>
<xml_diff>
--- a/data/Rationalisation score.xlsx
+++ b/data/Rationalisation score.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ErwinSiegers\Documents\GitHub\ssis-code-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ErwinSiegers\Documents\GitHub\ssis-code-parser\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476E683-0C14-406A-88E7-C4AAE66ED89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDCD07C-C439-4820-A770-B342AEEF0CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{520D7562-7803-464E-B711-1ACA2A639B0A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Rule</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>Flag</t>
+  </si>
+  <si>
+    <t>Bool</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Intercept</t>
   </si>
 </sst>
 </file>
@@ -540,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070AE968-799B-4E4E-9293-F8D0FC2639F6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +563,7 @@
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,128 +571,185 @@
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>-5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>-3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>-2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>-4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>-1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>-2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>-2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>-3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>-3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>